<commit_message>
Ajout de la BOM
</commit_message>
<xml_diff>
--- a/Afficheur temp/TEMP_BOM.xlsx
+++ b/Afficheur temp/TEMP_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\Tableau de bord\Carte élecs\Afficheur temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Dashboard_display\Afficheur temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20A708-15F0-4014-88C4-201266DF5A13}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED7C134-3543-4154-AD7F-CAE2BC93CE72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>